<commit_message>
Update developmental debt spreadsheet
</commit_message>
<xml_diff>
--- a/static/assets/xlsx/Developmental_Debt_Audit_Tool.xlsx
+++ b/static/assets/xlsx/Developmental_Debt_Audit_Tool.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Start Here" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="The Audit Ledger" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Examples" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Dashboard" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Start Here" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="The Audit Ledger" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Examples" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
+  <si>
+    <t xml:space="preserve">Global Governance Frameworks: Developmental Debt Audit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The bill is coming due. This is what you owe.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read the full manifesto: globalgovernanceframeworks.org/blog/the-bill-is-coming-due</t>
+  </si>
+  <si>
+    <t xml:space="preserve">⚠️ THE MARGIN CALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your Total Developmental Debt:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annual Avoidance Cost:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Future Cleanup Cost:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lost Opportunity Cost:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debt Breakdown by Stage:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue Debt (Rigidity):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate in Audit Ledger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orange Debt (Externalization):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green Debt (Paralysis):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEXT STEPS:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Go to "The Audit Ledger" tab and fill in your organizational debts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. See "Examples" tab for guidance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Return here to see your total exposure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Use this number in your strategic planning</t>
+  </si>
   <si>
     <t xml:space="preserve">Global Governance Frameworks: Developmental Debt Calculator</t>
   </si>
@@ -84,25 +139,70 @@
     <t xml:space="preserve">TOTAL DEBT ($)</t>
   </si>
   <si>
+    <t xml:space="preserve">What Happens If We Default?</t>
+  </si>
+  <si>
     <t xml:space="preserve">GRAND TOTAL DEBT:</t>
   </si>
   <si>
+    <t xml:space="preserve">Breakdown by Stage:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue Debt:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orange Debt:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green Debt:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default Scenario</t>
+  </si>
+  <si>
     <t xml:space="preserve">Blue Debt (Rigidity)</t>
   </si>
   <si>
     <t xml:space="preserve">Legacy IT System maintained to avoid upgrade pain</t>
   </si>
   <si>
+    <t xml:space="preserve">Technical bankruptcy when system fails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HR policies that ignore remote work reality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Talent exodus; inability to compete</t>
+  </si>
+  <si>
     <t xml:space="preserve">Orange Debt (Externalization)</t>
   </si>
   <si>
-    <t xml:space="preserve">Ignoring Supply Chain Carbon/Human Rights risks</t>
+    <t xml:space="preserve">Supply Chain carbon/human rights risks ignored</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regulatory fines, brand collapse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee burnout treated as normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mass turnover, institutional knowledge loss</t>
   </si>
   <si>
     <t xml:space="preserve">Green Debt (Paralysis)</t>
   </si>
   <si>
-    <t xml:space="preserve">Decision-making gridlock due to 'consensus' culture</t>
+    <t xml:space="preserve">Decision gridlock due to consensus culture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Market window closes, competitors move</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avoiding hard conversations about performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mediocrity becomes culture, A-players leave</t>
   </si>
 </sst>
 </file>
@@ -113,7 +213,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="\$#,##0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -154,8 +254,24 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="14"/>
+      <color rgb="FFC0392B"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="20"/>
+      <color rgb="FFC0392B"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -169,12 +285,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCF3CF"/>
+        <bgColor rgb="FFF2F3F4"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -189,7 +311,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -202,6 +324,13 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
       <diagonal/>
     </border>
   </borders>
@@ -230,7 +359,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -243,24 +372,28 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -292,8 +425,8 @@
       <rgbColor rgb="FF7F8C8D"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFCF3CF"/>
       <rgbColor rgb="FFF2F3F4"/>
-      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -326,7 +459,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFC0392B"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF2C3E50"/>
@@ -340,20 +473,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="145.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="20.71"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -363,7 +496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>2</v>
       </c>
@@ -372,58 +505,107 @@
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="B7" s="5" t="n">
+        <f aca="false">'The Audit Ledger'!F19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" s="0" t="s">
+      <c r="B9" s="6" t="n">
+        <f aca="false">'The Audit Ledger'!C19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="B10" s="6" t="n">
+        <f aca="false">'The Audit Ledger'!D19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" s="0" t="s">
+      <c r="B11" s="6" t="n">
+        <f aca="false">'The Audit Ledger'!E19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="0" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B8" s="0" t="s">
+      <c r="B15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="0" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B9" s="0" t="s">
+      <c r="B16" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="B17" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:D5"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" display="globalgovernanceframeworks.org/blog/the-bill-is-coming-due"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -439,162 +621,93 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:F14"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="80.71"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="3" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="3" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6" t="n">
-        <f aca="false">SUM(C4:E4)</f>
-        <v>0</v>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6" t="n">
-        <f aca="false">SUM(C5:E5)</f>
-        <v>0</v>
+      <c r="A5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6" t="n">
-        <f aca="false">SUM(C6:E6)</f>
-        <v>0</v>
+      <c r="A6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6" t="n">
-        <f aca="false">SUM(C7:E7)</f>
-        <v>0</v>
+      <c r="A7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6" t="n">
-        <f aca="false">SUM(C8:E8)</f>
-        <v>0</v>
+      <c r="A8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6" t="n">
-        <f aca="false">SUM(C9:E9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="6" t="n">
-        <f aca="false">SUM(C10:E10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6" t="n">
-        <f aca="false">SUM(C11:E11)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6" t="n">
-        <f aca="false">SUM(C12:E12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6" t="n">
-        <f aca="false">SUM(C13:E13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="7" t="n">
-        <f aca="false">SUM(F4:F13)</f>
-        <v>0</v>
+      <c r="A9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" display="globalgovernanceframeworks.org"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -610,10 +723,275 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:F5"/>
+  <dimension ref="A3:G24"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.81"/>
+  </cols>
+  <sheetData>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="6" t="n">
+        <f aca="false">SUM(C4:E4)</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="6" t="n">
+        <f aca="false">SUM(C5:E5)</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="6" t="n">
+        <f aca="false">SUM(C6:E6)</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="6" t="n">
+        <f aca="false">SUM(C7:E7)</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="6" t="n">
+        <f aca="false">SUM(C8:E8)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="6" t="n">
+        <f aca="false">SUM(C9:E9)</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="6" t="n">
+        <f aca="false">SUM(C10:E10)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="6" t="n">
+        <f aca="false">SUM(C11:E11)</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="6" t="n">
+        <f aca="false">SUM(C12:E12)</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="6" t="n">
+        <f aca="false">SUM(C13:E13)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="6" t="n">
+        <f aca="false">SUM(C14:E14)</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="6" t="n">
+        <f aca="false">SUM(C15:E15)</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="6" t="n">
+        <f aca="false">SUM(C16:E16)</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="6" t="n">
+        <f aca="false">SUM(C17:E17)</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="6" t="n">
+        <f aca="false">SUM(C18:E18)</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" customFormat="false" ht="24.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="5" t="n">
+        <f aca="false">SUM(F4:F18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:G8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -623,90 +1001,175 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="40.71"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="5" t="n">
+        <v>46</v>
+      </c>
+      <c r="C3" s="8" t="n">
         <v>500000</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3" s="8" t="n">
         <v>2000000</v>
       </c>
-      <c r="E3" s="5" t="n">
+      <c r="E3" s="8" t="n">
         <v>5000000</v>
       </c>
-      <c r="F3" s="5" t="n">
+      <c r="F3" s="8" t="n">
         <f aca="false">SUM(C3:E3)</f>
         <v>7500000</v>
       </c>
+      <c r="G3" s="7" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>150000</v>
-      </c>
-      <c r="D4" s="5" t="n">
-        <v>10000000</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5" t="n">
+        <v>48</v>
+      </c>
+      <c r="C4" s="8" t="n">
+        <v>300000</v>
+      </c>
+      <c r="D4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8" t="n">
+        <v>8000000</v>
+      </c>
+      <c r="F4" s="8" t="n">
         <f aca="false">SUM(C4:E4)</f>
-        <v>10150000</v>
+        <v>8300000</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="C5" s="8" t="n">
+        <v>150000</v>
+      </c>
+      <c r="D5" s="8" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="E5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8" t="n">
+        <f aca="false">SUM(C5:E5)</f>
+        <v>10150000</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="8" t="n">
+        <v>800000</v>
+      </c>
+      <c r="D6" s="8" t="n">
+        <v>5000000</v>
+      </c>
+      <c r="E6" s="8" t="n">
+        <v>12000000</v>
+      </c>
+      <c r="F6" s="8" t="n">
+        <f aca="false">SUM(C6:E6)</f>
+        <v>17800000</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="8" t="n">
         <v>1200000</v>
       </c>
-      <c r="D5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5" t="n">
+      <c r="D7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8" t="n">
         <v>3000000</v>
       </c>
-      <c r="F5" s="5" t="n">
-        <f aca="false">SUM(C5:E5)</f>
+      <c r="F7" s="8" t="n">
+        <f aca="false">SUM(C7:E7)</f>
         <v>4200000</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="8" t="n">
+        <v>400000</v>
+      </c>
+      <c r="D8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8" t="n">
+        <v>2000000</v>
+      </c>
+      <c r="F8" s="8" t="n">
+        <f aca="false">SUM(C8:E8)</f>
+        <v>2400000</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>